<commit_message>
Added XML and Json file writers and it`s logging
</commit_message>
<xml_diff>
--- a/src/main/resources/statisticsInfo.xlsx
+++ b/src/main/resources/statisticsInfo.xlsx
@@ -29,16 +29,16 @@
     <t>Названия университетов</t>
   </si>
   <si>
+    <t>LINGUISTICS</t>
+  </si>
+  <si>
+    <t>Воронежский Литературно-Переводческий Университет;</t>
+  </si>
+  <si>
     <t>PHYSICS</t>
   </si>
   <si>
     <t>Московский Выдуманный Университет;Московский Придуманный Институт;</t>
-  </si>
-  <si>
-    <t>LINGUISTICS</t>
-  </si>
-  <si>
-    <t>Воронежский Литературно-Переводческий Университет;</t>
   </si>
   <si>
     <t>MATHEMATICS</t>
@@ -134,13 +134,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>4.539999961853027</v>
+        <v>0.0</v>
       </c>
       <c r="C2" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="D2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -151,13 +151,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0</v>
+        <v>4.539999961853027</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="D3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>

</xml_diff>